<commit_message>
ex4: tab switch (load more reviews button is wrong in location)
</commit_message>
<xml_diff>
--- a/ex4/An-Phân tích sử dụng các thẻ tuần1 bài4.xlsx
+++ b/ex4/An-Phân tích sử dụng các thẻ tuần1 bài4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antv\Downloads\BaiTapFresherDev\Projects\antv-runs.github.io\ex4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F15DCA-A91C-45DC-9F49-99189471DF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2864AA17-8B3C-41CF-A2DA-50812DA508B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="1905" windowWidth="21120" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="600" windowWidth="25200" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>div (class="container")</t>
   </si>
@@ -39,12 +39,6 @@
     <t>button (class="tabs__tab")</t>
   </si>
   <si>
-    <t>section (class="reviews")</t>
-  </si>
-  <si>
-    <t>header (class="reviews__header")</t>
-  </si>
-  <si>
     <t>h2 (class="reviews__title")</t>
   </si>
   <si>
@@ -69,15 +63,6 @@
     <t>div (class="review-card__meta")</t>
   </si>
   <si>
-    <t>header (class="review-card__header")</t>
-  </si>
-  <si>
-    <t>div (class="review-card__content")</t>
-  </si>
-  <si>
-    <t>footer (class="review-card__footer")</t>
-  </si>
-  <si>
     <t>… &lt;li&gt; lặp lại</t>
   </si>
   <si>
@@ -109,6 +94,45 @@
   </si>
   <si>
     <t>body</t>
+  </si>
+  <si>
+    <t>section (class="product-tabs__content reviews")</t>
+  </si>
+  <si>
+    <t>div (class="review-card__header")</t>
+  </si>
+  <si>
+    <t>sửa</t>
+  </si>
+  <si>
+    <t>div (class="reviews__header")</t>
+  </si>
+  <si>
+    <t>đổi lại thành select-box</t>
+  </si>
+  <si>
+    <t>p (class="review-card__content")</t>
+  </si>
+  <si>
+    <t>p (class="review-card__footer")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Trang chỉ có 1 h1/ 1 header / 1 </t>
+  </si>
+  <si>
+    <t>vì chỉ là text bình thường nên dùng thẻ &lt;p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xem lại class: nếu common nhiều thì hãy đặt tên class chung </t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>có 4 thuộc tính chung nên đặt reviews__action được</t>
+  </si>
+  <si>
+    <t>đổi nút phía trên</t>
   </si>
 </sst>
 </file>
@@ -489,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="O3:U34"/>
+  <dimension ref="O3:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,14 +527,15 @@
     <col min="18" max="18" width="5.85546875" customWidth="1"/>
     <col min="19" max="19" width="5.5703125" customWidth="1"/>
     <col min="20" max="20" width="6.28515625" customWidth="1"/>
+    <col min="29" max="29" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="O3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P4" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +545,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
         <v>1</v>
@@ -530,7 +555,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1" t="s">
@@ -540,7 +565,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -550,7 +575,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -560,7 +585,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -570,220 +595,265 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-    </row>
-    <row r="12" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="AA11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="15:21" ht="21" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P26" s="1"/>
       <c r="Q26" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="16:21" ht="21" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="16:20" ht="21" x14ac:dyDescent="0.35">
@@ -792,14 +862,14 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="16:20" ht="21" x14ac:dyDescent="0.35">
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="T34" s="1"/>
     </row>

</xml_diff>

<commit_message>
ex4: use select box for latest button
</commit_message>
<xml_diff>
--- a/ex4/An-Phân tích sử dụng các thẻ tuần1 bài4.xlsx
+++ b/ex4/An-Phân tích sử dụng các thẻ tuần1 bài4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antv\Downloads\BaiTapFresherDev\Projects\antv-runs.github.io\ex4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2864AA17-8B3C-41CF-A2DA-50812DA508B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CB700C-EFC4-4F5E-98E8-88DA18174134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="600" windowWidth="25200" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="2010" windowWidth="22050" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>div (class="container")</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>đổi nút phía trên</t>
+  </si>
+  <si>
+    <t>dùng &lt;select&gt; nhưng không custom được các &lt;option&gt;</t>
   </si>
 </sst>
 </file>
@@ -515,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="O3:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +681,12 @@
       <c r="AD15" t="s">
         <v>35</v>
       </c>
+      <c r="AH15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="15:35" ht="21" x14ac:dyDescent="0.35">
       <c r="P16" s="1"/>

</xml_diff>

<commit_message>
[TL.Review] ex4 - layout
</commit_message>
<xml_diff>
--- a/ex4/An-Phân tích sử dụng các thẻ tuần1 bài4.xlsx
+++ b/ex4/An-Phân tích sử dụng các thẻ tuần1 bài4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antv\Downloads\BaiTapFresherDev\Projects\antv-runs.github.io\ex4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CB700C-EFC4-4F5E-98E8-88DA18174134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ED1F75-C8A1-4BD0-A02A-385D850A0F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2010" windowWidth="22050" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="2010" windowWidth="22050" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>div (class="container")</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>dùng &lt;select&gt; nhưng không custom được các &lt;option&gt;</t>
+  </si>
+  <si>
+    <t>tự đổi</t>
+  </si>
+  <si>
+    <t>thêm div bên ngoài</t>
   </si>
 </sst>
 </file>
@@ -518,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="O3:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,6 +804,12 @@
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
+      <c r="AA24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="16:31" ht="21" x14ac:dyDescent="0.35">
       <c r="P25" s="1"/>

</xml_diff>